<commit_message>
Update Top N script and code
Update Top N script and code
</commit_message>
<xml_diff>
--- a/Prequal Monitor Result - 21'03.xlsx
+++ b/Prequal Monitor Result - 21'03.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Git-hub.com Clone\Springboot-Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A1628AB-1321-42C2-B07F-EDE798D19100}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D02C4A0-80FC-4DE4-9550-4C6E43862B21}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="684" yWindow="180" windowWidth="21924" windowHeight="12012" tabRatio="461" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="163">
   <si>
     <t>Monitor Criteria</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -646,6 +646,22 @@
   </si>
   <si>
     <t>dataType||itemName||pointCount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>targetStartDate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>targetEndDate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>if blank =&gt; Now</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">mUT + 4 hr </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -780,27 +796,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -810,20 +805,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -836,6 +819,39 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1119,10 +1135,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AQ45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="AB1" sqref="AB1"/>
-      <selection pane="bottomLeft" activeCell="AO5" sqref="AO5"/>
+      <selection pane="bottomLeft" activeCell="AH30" sqref="AH30:AH39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1133,7 +1149,7 @@
     <col min="4" max="4" width="8.25" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.75" style="1" customWidth="1"/>
     <col min="6" max="6" width="28.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.25" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.5" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" style="1"/>
@@ -1174,222 +1190,222 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:43" x14ac:dyDescent="0.3">
-      <c r="B2" s="20"/>
-      <c r="C2" s="17" t="s">
+      <c r="B2" s="9"/>
+      <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="13" t="s">
+      <c r="D2" s="5"/>
+      <c r="E2" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="15"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="14"/>
       <c r="K2" s="2"/>
       <c r="L2" s="18" t="s">
         <v>0</v>
       </c>
       <c r="M2" s="18"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="13" t="s">
+      <c r="N2" s="5"/>
+      <c r="O2" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
-      <c r="S2" s="15"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
+      <c r="S2" s="14"/>
       <c r="U2" s="2"/>
-      <c r="V2" s="19" t="s">
+      <c r="V2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="W2" s="12"/>
-      <c r="X2" s="13" t="s">
+      <c r="W2" s="5"/>
+      <c r="X2" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="Y2" s="14"/>
-      <c r="Z2" s="14"/>
-      <c r="AA2" s="14"/>
-      <c r="AB2" s="15"/>
-      <c r="AD2" s="20"/>
+      <c r="Y2" s="13"/>
+      <c r="Z2" s="13"/>
+      <c r="AA2" s="13"/>
+      <c r="AB2" s="14"/>
+      <c r="AD2" s="9"/>
       <c r="AE2" s="18" t="s">
         <v>1</v>
       </c>
       <c r="AF2" s="18"/>
-      <c r="AG2" s="12"/>
-      <c r="AH2" s="13" t="s">
+      <c r="AG2" s="5"/>
+      <c r="AH2" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="AI2" s="14"/>
-      <c r="AJ2" s="14"/>
-      <c r="AK2" s="14"/>
-      <c r="AL2" s="15"/>
+      <c r="AI2" s="13"/>
+      <c r="AJ2" s="13"/>
+      <c r="AK2" s="13"/>
+      <c r="AL2" s="14"/>
     </row>
     <row r="3" spans="2:43" x14ac:dyDescent="0.3">
-      <c r="B3" s="20"/>
-      <c r="C3" s="17" t="s">
+      <c r="B3" s="9"/>
+      <c r="C3" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="H3" s="14"/>
-      <c r="I3" s="15"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="14"/>
       <c r="K3" s="2"/>
       <c r="L3" s="18" t="s">
         <v>54</v>
       </c>
       <c r="M3" s="18"/>
-      <c r="N3" s="12" t="s">
+      <c r="N3" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="O3" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="P3" s="16" t="s">
+      <c r="P3" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="Q3" s="13" t="s">
+      <c r="Q3" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="R3" s="14"/>
-      <c r="S3" s="15"/>
+      <c r="R3" s="13"/>
+      <c r="S3" s="14"/>
       <c r="U3" s="2"/>
-      <c r="V3" s="19" t="s">
+      <c r="V3" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="W3" s="12" t="s">
+      <c r="W3" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="X3" s="16" t="s">
+      <c r="X3" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="Y3" s="16" t="s">
+      <c r="Y3" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="Z3" s="13" t="s">
+      <c r="Z3" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="AA3" s="14"/>
-      <c r="AB3" s="15"/>
-      <c r="AD3" s="20"/>
-      <c r="AE3" s="19"/>
-      <c r="AF3" s="19"/>
-      <c r="AG3" s="12" t="s">
+      <c r="AA3" s="13"/>
+      <c r="AB3" s="14"/>
+      <c r="AD3" s="9"/>
+      <c r="AE3" s="8"/>
+      <c r="AF3" s="8"/>
+      <c r="AG3" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="AH3" s="16" t="s">
+      <c r="AH3" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="AI3" s="16" t="s">
+      <c r="AI3" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="AJ3" s="13" t="s">
+      <c r="AJ3" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="AK3" s="14"/>
-      <c r="AL3" s="15"/>
+      <c r="AK3" s="13"/>
+      <c r="AL3" s="14"/>
     </row>
     <row r="4" spans="2:43" x14ac:dyDescent="0.3">
-      <c r="B4" s="20"/>
-      <c r="C4" s="17" t="s">
+      <c r="B4" s="9"/>
+      <c r="C4" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16" t="s">
+      <c r="E4" s="6"/>
+      <c r="F4" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="16" t="s">
+      <c r="H4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="16" t="s">
+      <c r="I4" s="6" t="s">
         <v>87</v>
       </c>
       <c r="K4" s="2"/>
-      <c r="L4" s="19" t="s">
+      <c r="L4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="M4" s="19" t="s">
+      <c r="M4" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="N4" s="12" t="s">
+      <c r="N4" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="O4" s="16"/>
-      <c r="P4" s="16"/>
-      <c r="Q4" s="12" t="s">
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="R4" s="12" t="s">
+      <c r="R4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="S4" s="12" t="s">
+      <c r="S4" s="5" t="s">
         <v>87</v>
       </c>
       <c r="U4" s="2"/>
-      <c r="V4" s="19" t="s">
+      <c r="V4" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="W4" s="12" t="s">
+      <c r="W4" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="X4" s="16"/>
-      <c r="Y4" s="16"/>
-      <c r="Z4" s="12" t="s">
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
+      <c r="Z4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AA4" s="12" t="s">
+      <c r="AA4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="AB4" s="12" t="s">
+      <c r="AB4" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="AD4" s="20"/>
-      <c r="AE4" s="17" t="s">
+      <c r="AD4" s="9"/>
+      <c r="AE4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="AF4" s="17" t="s">
+      <c r="AF4" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="AG4" s="12" t="s">
+      <c r="AG4" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="AH4" s="16"/>
-      <c r="AI4" s="16"/>
-      <c r="AJ4" s="12" t="s">
+      <c r="AH4" s="6"/>
+      <c r="AI4" s="6"/>
+      <c r="AJ4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AK4" s="12" t="s">
+      <c r="AK4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="AL4" s="12" t="s">
+      <c r="AL4" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="AN4" s="21" t="s">
+      <c r="AN4" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="AO4" s="12" t="s">
+      <c r="AO4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AP4" s="12" t="s">
+      <c r="AP4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="AQ4" s="12" t="s">
+      <c r="AQ4" s="5" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1402,9 +1418,11 @@
         <v>120</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="F5" s="2"/>
+        <v>90</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -1435,15 +1453,15 @@
       <c r="X5" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="Y5" s="20" t="s">
+      <c r="Y5" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="Z5" s="4" t="s">
+      <c r="Z5" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="AA5" s="5"/>
-      <c r="AB5" s="6"/>
-      <c r="AD5" s="20"/>
+      <c r="AA5" s="20"/>
+      <c r="AB5" s="21"/>
+      <c r="AD5" s="9"/>
       <c r="AE5" s="2" t="s">
         <v>6</v>
       </c>
@@ -1466,7 +1484,7 @@
       <c r="AL5" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="AN5" s="21" t="s">
+      <c r="AN5" s="10" t="s">
         <v>151</v>
       </c>
       <c r="AO5" s="2" t="s">
@@ -1486,10 +1504,10 @@
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -1520,12 +1538,12 @@
       <c r="Y6" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="Z6" s="5" t="s">
+      <c r="Z6" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="AA6" s="5"/>
-      <c r="AB6" s="6"/>
-      <c r="AD6" s="20"/>
+      <c r="AA6" s="20"/>
+      <c r="AB6" s="21"/>
+      <c r="AD6" s="9"/>
       <c r="AE6" s="2" t="s">
         <v>25</v>
       </c>
@@ -1540,7 +1558,7 @@
       <c r="AJ6" s="2"/>
       <c r="AK6" s="2"/>
       <c r="AL6" s="2"/>
-      <c r="AN6" s="21" t="s">
+      <c r="AN6" s="10" t="s">
         <v>152</v>
       </c>
       <c r="AO6" s="2"/>
@@ -1558,11 +1576,9 @@
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>93</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -1591,7 +1607,7 @@
       <c r="Z7" s="2"/>
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
-      <c r="AD7" s="20"/>
+      <c r="AD7" s="9"/>
       <c r="AE7" s="2" t="s">
         <v>8</v>
       </c>
@@ -1606,7 +1622,7 @@
       <c r="AJ7" s="2"/>
       <c r="AK7" s="2"/>
       <c r="AL7" s="2"/>
-      <c r="AN7" s="21" t="s">
+      <c r="AN7" s="10" t="s">
         <v>153</v>
       </c>
       <c r="AO7" s="2"/>
@@ -1622,9 +1638,11 @@
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="F8" s="2"/>
+        <v>94</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
@@ -1649,7 +1667,7 @@
       <c r="Z8" s="2"/>
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
-      <c r="AD8" s="20"/>
+      <c r="AD8" s="9"/>
       <c r="AE8" s="2" t="s">
         <v>7</v>
       </c>
@@ -1670,10 +1688,10 @@
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -1699,7 +1717,7 @@
       <c r="Z9" s="2"/>
       <c r="AA9" s="2"/>
       <c r="AB9" s="2"/>
-      <c r="AD9" s="20"/>
+      <c r="AD9" s="9"/>
       <c r="AE9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1720,12 +1738,12 @@
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="G10" s="2"/>
+        <v>159</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2" t="s">
+        <v>121</v>
+      </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="K10" s="2"/>
@@ -1749,7 +1767,7 @@
       <c r="Z10" s="2"/>
       <c r="AA10" s="2"/>
       <c r="AB10" s="2"/>
-      <c r="AD10" s="20"/>
+      <c r="AD10" s="9"/>
       <c r="AE10" s="2" t="s">
         <v>11</v>
       </c>
@@ -1769,9 +1787,15 @@
         <v>62</v>
       </c>
       <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>162</v>
+      </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="K11" s="2"/>
@@ -1795,7 +1819,7 @@
       <c r="Z11" s="2"/>
       <c r="AA11" s="2"/>
       <c r="AB11" s="2"/>
-      <c r="AD11" s="20"/>
+      <c r="AD11" s="9"/>
       <c r="AE11" s="2" t="s">
         <v>10</v>
       </c>
@@ -1815,12 +1839,8 @@
         <v>63</v>
       </c>
       <c r="D12" s="2"/>
-      <c r="E12" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>108</v>
-      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -1845,7 +1865,7 @@
       <c r="Z12" s="2"/>
       <c r="AA12" s="2"/>
       <c r="AB12" s="2"/>
-      <c r="AD12" s="20"/>
+      <c r="AD12" s="9"/>
       <c r="AE12" s="2" t="s">
         <v>12</v>
       </c>
@@ -1864,18 +1884,18 @@
       <c r="C13" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="9"/>
+      <c r="E13" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2" t="s">
         <v>13</v>
@@ -1897,7 +1917,7 @@
       <c r="Z13" s="2"/>
       <c r="AA13" s="2"/>
       <c r="AB13" s="2"/>
-      <c r="AD13" s="20"/>
+      <c r="AD13" s="9"/>
       <c r="AE13" s="2" t="s">
         <v>13</v>
       </c>
@@ -1916,16 +1936,18 @@
       <c r="C14" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
+      <c r="D14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="17"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2" t="s">
         <v>18</v>
@@ -1949,7 +1971,7 @@
       <c r="V14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AD14" s="20"/>
+      <c r="AD14" s="9"/>
       <c r="AE14" s="2" t="s">
         <v>18</v>
       </c>
@@ -1972,13 +1994,13 @@
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="G15" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2" t="s">
@@ -1988,20 +2010,20 @@
         <v>19</v>
       </c>
       <c r="N15" s="2"/>
-      <c r="O15" s="10" t="s">
+      <c r="O15" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="P15" s="7" t="s">
+      <c r="P15" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="Q15" s="8"/>
-      <c r="R15" s="8"/>
-      <c r="S15" s="9"/>
+      <c r="Q15" s="16"/>
+      <c r="R15" s="16"/>
+      <c r="S15" s="17"/>
       <c r="U15" s="2"/>
       <c r="V15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="AD15" s="20"/>
+      <c r="AD15" s="9"/>
       <c r="AE15" s="2" t="s">
         <v>19</v>
       </c>
@@ -2028,12 +2050,12 @@
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="I16" s="2"/>
       <c r="K16" s="2"/>
@@ -2055,15 +2077,15 @@
       <c r="AE16" s="2"/>
       <c r="AF16" s="2"/>
       <c r="AG16" s="2"/>
-      <c r="AH16" s="10" t="s">
+      <c r="AH16" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="AI16" s="7" t="s">
+      <c r="AI16" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="AJ16" s="8"/>
-      <c r="AK16" s="8"/>
-      <c r="AL16" s="9"/>
+      <c r="AJ16" s="16"/>
+      <c r="AK16" s="16"/>
+      <c r="AL16" s="17"/>
     </row>
     <row r="17" spans="2:38" x14ac:dyDescent="0.3">
       <c r="B17" s="2"/>
@@ -2072,12 +2094,12 @@
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="I17" s="2"/>
       <c r="K17" s="2"/>
@@ -2116,12 +2138,12 @@
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2" t="s">
-        <v>103</v>
+        <v>29</v>
       </c>
       <c r="I18" s="2"/>
       <c r="K18" s="2" t="s">
@@ -2176,12 +2198,12 @@
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2" t="s">
-        <v>30</v>
+        <v>103</v>
       </c>
       <c r="I19" s="2"/>
       <c r="K19" s="2" t="s">
@@ -2234,12 +2256,12 @@
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="F20" s="11"/>
+        <v>114</v>
+      </c>
+      <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I20" s="2"/>
       <c r="K20" s="2"/>
@@ -2288,12 +2310,12 @@
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F21" s="2"/>
+        <v>115</v>
+      </c>
+      <c r="F21" s="4"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2" t="s">
-        <v>106</v>
+        <v>31</v>
       </c>
       <c r="I21" s="2"/>
       <c r="K21" s="2"/>
@@ -2342,14 +2364,14 @@
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="H22" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" s="2" t="s">
         <v>24</v>
@@ -2361,7 +2383,7 @@
       <c r="O22" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="P22" s="11"/>
+      <c r="P22" s="4"/>
       <c r="Q22" s="2"/>
       <c r="R22" s="2" t="s">
         <v>31</v>
@@ -2396,13 +2418,13 @@
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
@@ -2434,7 +2456,7 @@
       <c r="AH23" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="AI23" s="11"/>
+      <c r="AI23" s="4"/>
       <c r="AJ23" s="2"/>
       <c r="AK23" s="2" t="s">
         <v>31</v>
@@ -2448,13 +2470,13 @@
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2" t="s">
-        <v>107</v>
+        <v>22</v>
       </c>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
@@ -2499,11 +2521,15 @@
         <v>82</v>
       </c>
       <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
+      <c r="E25" s="2" t="s">
+        <v>119</v>
+      </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
+      <c r="I25" s="2" t="s">
+        <v>107</v>
+      </c>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
@@ -2597,12 +2623,12 @@
       <c r="O27" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="P27" s="20" t="s">
+      <c r="P27" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="Q27" s="4"/>
-      <c r="R27" s="5"/>
-      <c r="S27" s="6"/>
+      <c r="Q27" s="19"/>
+      <c r="R27" s="20"/>
+      <c r="S27" s="21"/>
       <c r="AD27" s="2"/>
       <c r="AE27" s="2"/>
       <c r="AF27" s="2" t="s">
@@ -2637,12 +2663,12 @@
       <c r="O28" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="P28" s="20" t="s">
+      <c r="P28" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="Q28" s="4"/>
-      <c r="R28" s="5"/>
-      <c r="S28" s="6"/>
+      <c r="Q28" s="19"/>
+      <c r="R28" s="20"/>
+      <c r="S28" s="21"/>
       <c r="AD28" s="2"/>
       <c r="AE28" s="2"/>
       <c r="AF28" s="2" t="s">
@@ -2652,14 +2678,14 @@
       <c r="AH28" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="AI28" s="20" t="s">
+      <c r="AI28" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="AJ28" s="3" t="s">
+      <c r="AJ28" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="AK28" s="3"/>
-      <c r="AL28" s="3"/>
+      <c r="AK28" s="11"/>
+      <c r="AL28" s="11"/>
     </row>
     <row r="29" spans="2:38" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B29" s="2"/>
@@ -2690,14 +2716,14 @@
       <c r="AH29" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="AI29" s="20" t="s">
+      <c r="AI29" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="AJ29" s="3" t="s">
+      <c r="AJ29" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="AK29" s="3"/>
-      <c r="AL29" s="3"/>
+      <c r="AK29" s="11"/>
+      <c r="AL29" s="11"/>
     </row>
     <row r="30" spans="2:38" x14ac:dyDescent="0.3">
       <c r="B30" s="2"/>
@@ -2975,12 +3001,12 @@
       <c r="AH39" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="AI39" s="3" t="s">
+      <c r="AI39" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="AJ39" s="3"/>
-      <c r="AK39" s="3"/>
-      <c r="AL39" s="3"/>
+      <c r="AJ39" s="11"/>
+      <c r="AK39" s="11"/>
+      <c r="AL39" s="11"/>
     </row>
     <row r="40" spans="2:38" x14ac:dyDescent="0.3">
       <c r="B40" s="2"/>
@@ -3006,6 +3032,12 @@
       <c r="AL40" s="2"/>
     </row>
     <row r="41" spans="2:38" x14ac:dyDescent="0.3">
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
       <c r="AD41" s="2"/>
       <c r="AE41" s="2"/>
       <c r="AF41" s="2"/>
@@ -3071,11 +3103,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="AI39:AL39"/>
-    <mergeCell ref="AH2:AL2"/>
-    <mergeCell ref="AJ3:AL3"/>
-    <mergeCell ref="AI16:AL16"/>
-    <mergeCell ref="AE2:AF2"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="L2:M2"/>
     <mergeCell ref="Q27:S27"/>
     <mergeCell ref="Q28:S28"/>
     <mergeCell ref="AJ28:AL28"/>
@@ -3084,14 +3116,14 @@
     <mergeCell ref="Z3:AB3"/>
     <mergeCell ref="Z5:AB5"/>
     <mergeCell ref="Z6:AB6"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="L2:M2"/>
     <mergeCell ref="P15:S15"/>
     <mergeCell ref="O2:S2"/>
     <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="AI39:AL39"/>
+    <mergeCell ref="AH2:AL2"/>
+    <mergeCell ref="AJ3:AL3"/>
+    <mergeCell ref="AI16:AL16"/>
+    <mergeCell ref="AE2:AF2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>